<commit_message>
Update back to school simulation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -445,16 +445,16 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>0.1400000000000006</v>
+        <v>2.359999999999999</v>
       </c>
       <c r="D2">
-        <v>2.561275</v>
+        <v>2.5025</v>
       </c>
       <c r="E2">
-        <v>1.458575</v>
+        <v>0.56725</v>
       </c>
       <c r="F2">
-        <v>2.116875</v>
+        <v>1.62425</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -468,13 +468,13 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2.435275</v>
+        <v>2.477575</v>
       </c>
       <c r="E3">
-        <v>15.6917</v>
+        <v>2.7576</v>
       </c>
       <c r="F3">
-        <v>7.86085</v>
+        <v>2.6373</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -488,13 +488,13 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>2.05525</v>
+        <v>2.416075</v>
       </c>
       <c r="E4">
-        <v>60.293675</v>
+        <v>8.63185</v>
       </c>
       <c r="F4">
-        <v>26.3553</v>
+        <v>4.928575</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -505,16 +505,16 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>0.01999999999999602</v>
+        <v>0.9599999999999937</v>
       </c>
       <c r="D5">
-        <v>3.33276</v>
+        <v>3.29392</v>
       </c>
       <c r="E5">
-        <v>4.5636</v>
+        <v>1.34528</v>
       </c>
       <c r="F5">
-        <v>4.05548</v>
+        <v>2.47568</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -528,13 +528,13 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>2.62908</v>
+        <v>3.19428</v>
       </c>
       <c r="E6">
-        <v>67.2234</v>
+        <v>9.195320000000001</v>
       </c>
       <c r="F6">
-        <v>30.9076</v>
+        <v>5.800120000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -548,13 +548,13 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1.91988</v>
+        <v>2.97404</v>
       </c>
       <c r="E7">
-        <v>96.91308000000001</v>
+        <v>34.38672</v>
       </c>
       <c r="F7">
-        <v>58.64279999999999</v>
+        <v>14.94092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update model with recovered individuals
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+  <si>
+    <t>Community Infection Rate (per million)</t>
+  </si>
   <si>
     <t>School</t>
   </si>
@@ -408,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,7 +420,7 @@
     <col min="10" max="16" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -436,125 +439,284 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1600</v>
+      </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>2.359999999999999</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>2.5025</v>
+        <v>0.8499999999999943</v>
       </c>
       <c r="E2">
-        <v>0.56725</v>
+        <v>2.7912625</v>
       </c>
       <c r="F2">
-        <v>1.62425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>6</v>
+        <v>0.7550875</v>
+      </c>
+      <c r="G2">
+        <v>1.910325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1600</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>2.477575</v>
-      </c>
       <c r="E3">
-        <v>2.7576</v>
+        <v>2.7537625</v>
       </c>
       <c r="F3">
-        <v>2.6373</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>6</v>
+        <v>4.21895</v>
+      </c>
+      <c r="G3">
+        <v>3.51495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>1600</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>2.416075</v>
-      </c>
       <c r="E4">
-        <v>8.63185</v>
+        <v>2.6757125</v>
       </c>
       <c r="F4">
-        <v>4.928575</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>7</v>
+        <v>15.4135125</v>
+      </c>
+      <c r="G4">
+        <v>7.734450000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>1600</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>0.9599999999999937</v>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>3.29392</v>
+        <v>2.730000000000004</v>
       </c>
       <c r="E5">
-        <v>1.34528</v>
+        <v>2.972760000000001</v>
       </c>
       <c r="F5">
-        <v>2.47568</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+        <v>0.9780200000000001</v>
+      </c>
+      <c r="G5">
+        <v>2.103400000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>1600</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0.01000000000000512</v>
+      </c>
+      <c r="E6">
+        <v>2.94166</v>
+      </c>
+      <c r="F6">
+        <v>5.8306</v>
+      </c>
+      <c r="G6">
+        <v>4.24816</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>1600</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2.8132</v>
+      </c>
+      <c r="F7">
+        <v>20.97696</v>
+      </c>
+      <c r="G7">
+        <v>9.663779999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>400</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>3.19428</v>
-      </c>
-      <c r="E6">
-        <v>9.195320000000001</v>
-      </c>
-      <c r="F6">
-        <v>5.800120000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="D8">
+        <v>32.11999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.6792125</v>
+      </c>
+      <c r="F8">
+        <v>0.1878625</v>
+      </c>
+      <c r="G8">
+        <v>0.4564875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>400</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>2.97404</v>
-      </c>
-      <c r="E7">
-        <v>34.38672</v>
-      </c>
-      <c r="F7">
-        <v>14.94092</v>
+      <c r="D9">
+        <v>7.849999999999994</v>
+      </c>
+      <c r="E9">
+        <v>0.6730625</v>
+      </c>
+      <c r="F9">
+        <v>1.0128875</v>
+      </c>
+      <c r="G9">
+        <v>0.8268875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>400</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>2.939999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.66625</v>
+      </c>
+      <c r="F10">
+        <v>3.9106375</v>
+      </c>
+      <c r="G10">
+        <v>1.8469375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>400</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>39.97999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.75442</v>
+      </c>
+      <c r="F11">
+        <v>0.25372</v>
+      </c>
+      <c r="G11">
+        <v>0.5325800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>400</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>13.01000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0.74782</v>
+      </c>
+      <c r="F12">
+        <v>1.53048</v>
+      </c>
+      <c r="G12">
+        <v>1.08858</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>400</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>6.969999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.7417000000000001</v>
+      </c>
+      <c r="F13">
+        <v>6.161840000000001</v>
+      </c>
+      <c r="G13">
+        <v>2.65992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add scenarios for higher vaccination coverage
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
   <si>
     <t>Community Infection Rate (per million)</t>
   </si>
@@ -22,6 +22,9 @@
     <t>School</t>
   </si>
   <si>
+    <t>Vaccination Coverage (teachers / students)</t>
+  </si>
+  <si>
     <t>Mask wearing</t>
   </si>
   <si>
@@ -43,6 +46,18 @@
     <t>elementary</t>
   </si>
   <si>
+    <t>60% / 30%</t>
+  </si>
+  <si>
+    <t>60% / 0%</t>
+  </si>
+  <si>
+    <t>90% / 60%</t>
+  </si>
+  <si>
+    <t>90% / 0%</t>
+  </si>
+  <si>
     <t>with_mask</t>
   </si>
   <si>
@@ -70,6 +85,15 @@
     <t>2.8 [1.6, 4.2]</t>
   </si>
   <si>
+    <t>2.5 [1.5, 3.6]</t>
+  </si>
+  <si>
+    <t>2.4 [1.5, 3.5]</t>
+  </si>
+  <si>
+    <t>3.0 [1.6, 4.4]</t>
+  </si>
+  <si>
     <t>0.7 [0.2, 1.2]</t>
   </si>
   <si>
@@ -82,6 +106,12 @@
     <t>0.7 [0.2, 1.6]</t>
   </si>
   <si>
+    <t>0.6 [0.1, 1.1]</t>
+  </si>
+  <si>
+    <t>0.6 [0.1, 1.2]</t>
+  </si>
+  <si>
     <t>0.8 [0.1, 1.8]</t>
   </si>
   <si>
@@ -94,10 +124,25 @@
     <t>1.0 [0.0, 2.4]</t>
   </si>
   <si>
-    <t>5.8 [1.4, 12.8]</t>
-  </si>
-  <si>
-    <t>21.0 [5.4, 41.0]</t>
+    <t>5.8 [1.2, 12.6]</t>
+  </si>
+  <si>
+    <t>21.2 [5.2, 41.8]</t>
+  </si>
+  <si>
+    <t>0.5 [0.0, 1.2]</t>
+  </si>
+  <si>
+    <t>2.2 [0.6, 4.8]</t>
+  </si>
+  <si>
+    <t>6.4 [1.9, 13.0]</t>
+  </si>
+  <si>
+    <t>5.6 [1.2, 12.2]</t>
+  </si>
+  <si>
+    <t>19.7 [5.0, 39.6]</t>
   </si>
   <si>
     <t>0.2 [0.0, 0.8]</t>
@@ -109,13 +154,25 @@
     <t>3.9 [0.0, 13.0]</t>
   </si>
   <si>
-    <t>0.3 [0.0, 1.2]</t>
+    <t>0.2 [0.0, 1.2]</t>
   </si>
   <si>
     <t>1.5 [0.0, 5.8]</t>
   </si>
   <si>
-    <t>6.2 [0.0, 21.6]</t>
+    <t>6.2 [0.0, 22.0]</t>
+  </si>
+  <si>
+    <t>0.1 [0.0, 0.5]</t>
+  </si>
+  <si>
+    <t>0.5 [0.0, 1.9]</t>
+  </si>
+  <si>
+    <t>1.5 [0.0, 5.6]</t>
+  </si>
+  <si>
+    <t>5.5 [0.0, 19.8]</t>
   </si>
   <si>
     <t>1.9 [1.0, 3.0]</t>
@@ -130,7 +187,25 @@
     <t>2.1 [0.8, 3.8]</t>
   </si>
   <si>
-    <t>9.7 [2.8, 19.2]</t>
+    <t>4.2 [1.4, 8.2]</t>
+  </si>
+  <si>
+    <t>9.8 [2.6, 19.6]</t>
+  </si>
+  <si>
+    <t>1.6 [0.8, 2.6]</t>
+  </si>
+  <si>
+    <t>2.5 [1.1, 4.2]</t>
+  </si>
+  <si>
+    <t>4.2 [1.6, 7.8]</t>
+  </si>
+  <si>
+    <t>4.1 [1.4, 8.0]</t>
+  </si>
+  <si>
+    <t>9.3 [2.6, 18.8]</t>
   </si>
   <si>
     <t>0.5 [0.0, 1.1]</t>
@@ -145,10 +220,25 @@
     <t>0.5 [0.0, 1.4]</t>
   </si>
   <si>
+    <t>1.1 [0.0, 3.6]</t>
+  </si>
+  <si>
+    <t>2.7 [0.0, 9.2]</t>
+  </si>
+  <si>
+    <t>0.4 [0.0, 0.9]</t>
+  </si>
+  <si>
+    <t>0.6 [0.0, 1.5]</t>
+  </si>
+  <si>
+    <t>1.0 [0.0, 3.0]</t>
+  </si>
+  <si>
     <t>1.1 [0.0, 3.4]</t>
   </si>
   <si>
-    <t>2.7 [0.0, 9.4]</t>
+    <t>2.4 [0.0, 8.6]</t>
   </si>
 </sst>
 </file>
@@ -510,7 +600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -519,7 +609,7 @@
     <col min="10" max="16" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -541,281 +631,632 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1600</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
         <v>0.8499999999999943</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1600</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1600</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1600</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>2.730000000000004</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>2.549999999999997</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>1600</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>0.01000000000000512</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0.04999999999999716</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>1600</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>0.01000000000000512</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>1600</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>3.97999999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>1600</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>0.01999999999999602</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>1600</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>1600</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>3.019999999999996</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>1600</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>0.01999999999999602</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>1600</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>0.01999999999999602</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>400</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>32.11999999999999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>400</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>7.849999999999994</v>
+      </c>
+      <c r="F15" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
         <v>400</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>2.939999999999998</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>400</v>
+      </c>
+      <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="D8">
-        <v>32.11999999999999</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>40.45</v>
+      </c>
+      <c r="F17" t="s">
         <v>28</v>
       </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
         <v>400</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>7.849999999999994</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>13.20999999999999</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>400</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>6.839999999999989</v>
+      </c>
+      <c r="F19" t="s">
         <v>29</v>
       </c>
-      <c r="G9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
         <v>400</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>2.939999999999998</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>46.42999999999999</v>
+      </c>
+      <c r="F20" t="s">
         <v>30</v>
       </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
         <v>400</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>15.67</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>400</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>7.109999999999999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>400</v>
+      </c>
+      <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="D11">
-        <v>39.97999999999999</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23">
+        <v>40.95999999999999</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
         <v>400</v>
       </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>13.01000000000001</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>13.77999999999999</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
         <v>400</v>
       </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13">
-        <v>6.969999999999999</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" t="s">
-        <v>44</v>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>7.890000000000001</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>